<commit_message>
fix user project subsys compile port mis-match (with fsic) issue
</commit_message>
<xml_diff>
--- a/rtl/user/doc/user_project_wrapper.xlsx
+++ b/rtl/user/doc/user_project_wrapper.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="79">
   <si>
     <t xml:space="preserve">Keyword Name</t>
   </si>
@@ -307,8 +307,8 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">user_irq 
-hi_pri_req</t>
+    <t xml:space="preserve">low__pri_irq 
+High_pri_req</t>
   </si>
   <si>
     <t xml:space="preserve">la_data_o / la_data_0 :64</t>
@@ -367,6 +367,10 @@
 m_tlast </t>
   </si>
   <si>
+    <t xml:space="preserve">low__pri_irq ,
+high_pri_irq</t>
+  </si>
+  <si>
     <t xml:space="preserve">up_la_data:64</t>
   </si>
   <si>
@@ -385,10 +389,10 @@
     <t xml:space="preserve">ADD_PRI_PORT: axis_rst_n</t>
   </si>
   <si>
-    <t xml:space="preserve">ADD_PRI_PORT: USER_CLK2</t>
+    <t xml:space="preserve">ADD_PRI_PORT: user_clock2</t>
   </si>
   <si>
-    <t xml:space="preserve">ADD_PRI_PORT: USER_PRJ_SEL:2</t>
+    <t xml:space="preserve">ADD_PRI_PORT: user_prj_sel:5</t>
   </si>
   <si>
     <t xml:space="preserve">pADDR_WIDTH=10
@@ -733,7 +737,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.73"/>
@@ -873,11 +877,11 @@
   </sheetPr>
   <dimension ref="A1:J1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="27.12"/>
@@ -1223,15 +1227,15 @@
         <v>68</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>14</v>
@@ -1249,10 +1253,10 @@
         <v>14</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H18" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I18" s="26" t="s">
         <v>14</v>
@@ -1263,10 +1267,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>72</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>71</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>14</v>
@@ -1287,7 +1291,7 @@
         <v>14</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J19" s="28" t="s">
         <v>14</v>
@@ -1295,7 +1299,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>14</v>
@@ -1327,10 +1331,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>14</v>
@@ -1359,10 +1363,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>14</v>
@@ -1377,36 +1381,36 @@
         <v>14</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B23" s="26" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G23" s="26" t="s">
         <v>14</v>
@@ -1447,7 +1451,7 @@
         <v>29</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
fix port width mismatch issue between FSIC and USER SubSys
</commit_message>
<xml_diff>
--- a/rtl/user/doc/user_project_wrapper.xlsx
+++ b/rtl/user/doc/user_project_wrapper.xlsx
@@ -328,7 +328,7 @@
 axi_arvalid
 axi_araddr:pADDR_WIDTH
 axi_wvalid
-axi_wstrb 
+axi_wstrb :4
 axi_wdata:pDATA_WIDTH
 axi_rready
 cc_up_enable </t>
@@ -737,7 +737,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.73"/>
@@ -878,10 +878,10 @@
   <dimension ref="A1:J1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="27.12"/>

</xml_diff>

<commit_message>
clean up user_subsys database
</commit_message>
<xml_diff>
--- a/rtl/user/doc/user_project_wrapper.xlsx
+++ b/rtl/user/doc/user_project_wrapper.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="80">
   <si>
     <t xml:space="preserve">Keyword Name</t>
   </si>
@@ -374,25 +374,168 @@
     <t xml:space="preserve">up_la_data:64</t>
   </si>
   <si>
-    <t xml:space="preserve">ADD_PRI_PORT: axi_clk</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ADD_PRI_PORT: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">axi_clk</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">ADD_PRI_PORT: axis_clk</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ADD_PRI_PORT: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">axis_clk</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">ADD_PRI_PORT: axi_reset_n</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ADD_PRI_PORT: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">axi_reset_n</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">ADD_PRI_PORT: axis_rst_n</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ADD_PRI_PORT: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">axis_rst_n</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">ADD_PRI_PORT: user_clock2</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ADD_PRI_PORT: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">user_clock2</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">ADD_PRI_PORT: user_prj_sel:5</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ADD_PRI_PORT: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">uck2_rst_n</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ADD_PRI_PORT: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">user_prj_sel:5</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">pADDR_WIDTH=10
@@ -737,7 +880,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.73"/>
@@ -875,13 +1018,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1001"/>
+  <dimension ref="A1:J1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="27.12"/>
@@ -1397,77 +1540,97 @@
       <c r="A23" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="D23" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="H23" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="I23" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="J23" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="G23" s="26" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="26" t="s">
+      <c r="C24" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="26" t="s">
+      <c r="H24" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="J23" s="26" t="s">
+      <c r="I24" s="26" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="s">
+      <c r="J24" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H24" s="12" t="s">
+      <c r="H25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="I24" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J24" s="12" t="s">
+      <c r="I25" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J25" s="12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="9"/>
@@ -13181,6 +13344,18 @@
       <c r="I1001" s="10"/>
       <c r="J1001" s="10"/>
     </row>
+    <row r="1002" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1002" s="9"/>
+      <c r="B1002" s="10"/>
+      <c r="C1002" s="10"/>
+      <c r="D1002" s="10"/>
+      <c r="E1002" s="10"/>
+      <c r="F1002" s="10"/>
+      <c r="G1002" s="10"/>
+      <c r="H1002" s="10"/>
+      <c r="I1002" s="10"/>
+      <c r="J1002" s="10"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fix address width issue in user-subsys
</commit_message>
<xml_diff>
--- a/rtl/user/doc/user_project_wrapper.xlsx
+++ b/rtl/user/doc/user_project_wrapper.xlsx
@@ -190,10 +190,10 @@
   </si>
   <si>
     <t xml:space="preserve">awvalid_0 / awvalid,
-awaddr : pADDR_WIDTH,
+awaddr : 12,
 arvalid_0 / arvalid,
-araddr: pADDR_WIDTH,
-Wvalid_0 / wvalid, 
+araddr: 12,   
+wvalid_0 / wvalid, 
 wstrb_0 / wstrb: 4,  
 wdata : pDATA_WIDTH
 rready
@@ -218,9 +218,9 @@
   </si>
   <si>
     <t xml:space="preserve">awvalid_1 / awvalid
-awaddr : pADDR_WIDTH
-arvalid_1 / arvalid
-araddr: pADDR_WIDTH
+awaddr : 12
+arvalid_1 / arvalid 
+araddr: 12
 wvalid_1 / wvalid
 wstrb_1 / wstrb : 4,  
 wdata : pDATA_WIDTH,
@@ -237,9 +237,9 @@
   </si>
   <si>
     <t xml:space="preserve">awvalid_2 / awvalid
-awaddr : pADDR_WIDTH
-arvalid_2 / arvalid
-araddr: pADDR_WIDTH
+awaddr : 12
+arvalid_2 / arvalid 
+araddr: 12
 wvalid_2 / wvalid
 wstrb_2 / wstrb: 4, 
 wdata : pDATA_WIDTH
@@ -259,9 +259,9 @@
   </si>
   <si>
     <t xml:space="preserve">awvalid_3 / awvalid
-awaddr : pADDR_WIDTH
-arvalid_3 / arvalid
-araddr: pADDR_WIDTH
+awaddr : 12
+arvalid_3 / arvalid 
+araddr: 12
 wvalid_3 / wvalid
 wstrb_3 / wstrb :4  
 wdata : pDATA_WIDTH
@@ -324,9 +324,9 @@
   </si>
   <si>
     <t xml:space="preserve">axi_awvalid
-axi_awaddr:pADDR_WIDTH
+axi_awaddr : 15
 axi_arvalid
-axi_araddr:pADDR_WIDTH
+axi_araddr : 15
 axi_wvalid
 axi_wstrb :4
 axi_wdata:pDATA_WIDTH
@@ -880,7 +880,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.73"/>
@@ -1020,14 +1020,15 @@
   </sheetPr>
   <dimension ref="A1:J1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="17.38"/>

</xml_diff>